<commit_message>
add job offer skills to Job Offers
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Applicants" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="91">
   <si>
     <t>Creativity</t>
   </si>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1016,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1031,7 +1031,7 @@
     <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1044,10 +1044,20 @@
       <c r="D1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1060,8 +1070,17 @@
       <c r="D2" s="3">
         <v>44027</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1074,8 +1093,17 @@
       <c r="D3" s="3">
         <v>44028</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1088,8 +1116,20 @@
       <c r="D4" s="3">
         <v>44032</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1102,8 +1142,14 @@
       <c r="D5" s="3">
         <v>44032</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1116,8 +1162,14 @@
       <c r="D6" s="3">
         <v>44031</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -1130,8 +1182,14 @@
       <c r="D7" s="3">
         <v>44030</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -1144,8 +1202,17 @@
       <c r="D8" s="3">
         <v>44031</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -1158,8 +1225,20 @@
       <c r="D9" s="3">
         <v>44028</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1172,8 +1251,17 @@
       <c r="D10" s="3">
         <v>44031</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -1186,8 +1274,17 @@
       <c r="D11" s="3">
         <v>44031</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -1200,8 +1297,17 @@
       <c r="D12" s="3">
         <v>44028</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -1214,8 +1320,14 @@
       <c r="D13" s="3">
         <v>44027</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -1227,6 +1339,18 @@
       </c>
       <c r="D14" s="3">
         <v>44032</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1238,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:B64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update methods : reporter not matched , add exceptions
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Applicants" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="91">
   <si>
     <t>Creativity</t>
   </si>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1016,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1031,7 +1031,7 @@
     <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1044,10 +1044,20 @@
       <c r="D1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1060,8 +1070,17 @@
       <c r="D2" s="3">
         <v>44027</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1074,8 +1093,17 @@
       <c r="D3" s="3">
         <v>44028</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1088,8 +1116,20 @@
       <c r="D4" s="3">
         <v>44032</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1102,8 +1142,14 @@
       <c r="D5" s="3">
         <v>44032</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1116,8 +1162,14 @@
       <c r="D6" s="3">
         <v>44031</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -1130,8 +1182,14 @@
       <c r="D7" s="3">
         <v>44030</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -1144,8 +1202,17 @@
       <c r="D8" s="3">
         <v>44031</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -1158,8 +1225,20 @@
       <c r="D9" s="3">
         <v>44028</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -1172,8 +1251,17 @@
       <c r="D10" s="3">
         <v>44031</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -1186,8 +1274,17 @@
       <c r="D11" s="3">
         <v>44031</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -1200,8 +1297,17 @@
       <c r="D12" s="3">
         <v>44028</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -1214,8 +1320,14 @@
       <c r="D13" s="3">
         <v>44027</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -1227,6 +1339,18 @@
       </c>
       <c r="D14" s="3">
         <v>44032</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1238,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:B64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Formatting all code and add Reader Controller
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Applicants" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="135">
   <si>
     <t>Creativity</t>
   </si>
@@ -244,9 +244,6 @@
     <t>Offer Date</t>
   </si>
   <si>
-    <t>Agile Actors</t>
-  </si>
-  <si>
     <t>Java Developer</t>
   </si>
   <si>
@@ -305,6 +302,141 @@
   </si>
   <si>
     <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Thanasis</t>
+  </si>
+  <si>
+    <t>Athanasiou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 Argiroupoleos str., </t>
+  </si>
+  <si>
+    <t>athansiou@yahoo.gr</t>
+  </si>
+  <si>
+    <t>Panagiota</t>
+  </si>
+  <si>
+    <t>Panagiotou</t>
+  </si>
+  <si>
+    <t>24 Alimou str.,</t>
+  </si>
+  <si>
+    <t>panagiotou@outlook.com</t>
+  </si>
+  <si>
+    <t>Elisavet</t>
+  </si>
+  <si>
+    <t>Elisavetianou</t>
+  </si>
+  <si>
+    <t>61 Korai str.,</t>
+  </si>
+  <si>
+    <t>elisavet@hotmail.com</t>
+  </si>
+  <si>
+    <t>Christiana</t>
+  </si>
+  <si>
+    <t>Christou</t>
+  </si>
+  <si>
+    <t>4 Davleias str.,</t>
+  </si>
+  <si>
+    <t>christou@yahoo.com</t>
+  </si>
+  <si>
+    <t>Actors</t>
+  </si>
+  <si>
+    <t>Marios</t>
+  </si>
+  <si>
+    <t>Mariou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 Alimou str., </t>
+  </si>
+  <si>
+    <t>Lamia</t>
+  </si>
+  <si>
+    <t>mariou@hotmail.gr</t>
+  </si>
+  <si>
+    <t>Vagelis</t>
+  </si>
+  <si>
+    <t>Evagellou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 Katerinis str., </t>
+  </si>
+  <si>
+    <t>Katerini</t>
+  </si>
+  <si>
+    <t>vagelis@gmail.gr</t>
+  </si>
+  <si>
+    <t>Christos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99 Livadias str., </t>
+  </si>
+  <si>
+    <t>Livadia</t>
+  </si>
+  <si>
+    <t>chris@gmail.com</t>
+  </si>
+  <si>
+    <t>Arximidis</t>
+  </si>
+  <si>
+    <t>Arximidou</t>
+  </si>
+  <si>
+    <t>Drama</t>
+  </si>
+  <si>
+    <t>arximidis@yahoo.ger</t>
+  </si>
+  <si>
+    <t>Menelaos</t>
+  </si>
+  <si>
+    <t>Menelaou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Menidiou str., </t>
+  </si>
+  <si>
+    <t>men@gmail.com</t>
+  </si>
+  <si>
+    <t>Eleni</t>
+  </si>
+  <si>
+    <t>Eleniou</t>
+  </si>
+  <si>
+    <t>1 Lemessou str.,</t>
+  </si>
+  <si>
+    <t>489 Thivon str.,</t>
+  </si>
+  <si>
+    <t>Thiva</t>
+  </si>
+  <si>
+    <t>eleni@outlook.com</t>
   </si>
 </sst>
 </file>
@@ -693,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G10"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,7 +862,7 @@
         <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>65</v>
@@ -759,7 +891,7 @@
         <v>28</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F2" s="5">
         <v>34458</v>
@@ -791,7 +923,7 @@
         <v>28</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F3" s="5">
         <v>31614</v>
@@ -820,7 +952,7 @@
         <v>28</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F4" s="5">
         <v>28877</v>
@@ -846,10 +978,10 @@
         <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="5">
         <v>30886</v>
@@ -859,6 +991,9 @@
       </c>
       <c r="H5" t="s">
         <v>59</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -875,7 +1010,7 @@
         <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="5">
         <v>36304</v>
@@ -904,7 +1039,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F7" s="5">
         <v>35394</v>
@@ -917,6 +1052,9 @@
       </c>
       <c r="I7" t="s">
         <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -933,7 +1071,7 @@
         <v>28</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F8" s="5">
         <v>34069</v>
@@ -943,6 +1081,9 @@
       </c>
       <c r="H8" t="s">
         <v>52</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -956,10 +1097,10 @@
         <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F9" s="5">
         <v>33282</v>
@@ -971,7 +1112,7 @@
         <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -988,13 +1129,324 @@
         <v>28</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F10" s="5">
         <v>34482</v>
       </c>
       <c r="G10" t="s">
         <v>36</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="3">
+        <v>30695</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="3">
+        <v>35327</v>
+      </c>
+      <c r="G12" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="3">
+        <v>33115</v>
+      </c>
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="3">
+        <v>31847</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="3">
+        <v>34700</v>
+      </c>
+      <c r="G15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" s="3">
+        <v>29282</v>
+      </c>
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F17" s="3">
+        <v>35679</v>
+      </c>
+      <c r="G17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" s="3">
+        <v>29960</v>
+      </c>
+      <c r="G18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" s="3">
+        <v>32269</v>
+      </c>
+      <c r="G19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" s="3">
+        <v>36015</v>
+      </c>
+      <c r="G20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1008,18 +1460,28 @@
     <hyperlink ref="E8" r:id="rId7"/>
     <hyperlink ref="E10" r:id="rId8"/>
     <hyperlink ref="E9" r:id="rId9"/>
+    <hyperlink ref="E11" r:id="rId10"/>
+    <hyperlink ref="E12" r:id="rId11"/>
+    <hyperlink ref="E13" r:id="rId12"/>
+    <hyperlink ref="E14" r:id="rId13"/>
+    <hyperlink ref="E15" r:id="rId14"/>
+    <hyperlink ref="E16" r:id="rId15"/>
+    <hyperlink ref="E17" r:id="rId16"/>
+    <hyperlink ref="E18" r:id="rId17"/>
+    <hyperlink ref="E19" r:id="rId18"/>
+    <hyperlink ref="E20" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,7 +1530,7 @@
         <v>28</v>
       </c>
       <c r="D2" s="3">
-        <v>44027</v>
+        <v>43997</v>
       </c>
       <c r="E2" t="s">
         <v>66</v>
@@ -1091,7 +1553,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="3">
-        <v>44028</v>
+        <v>44018</v>
       </c>
       <c r="E3" t="s">
         <v>66</v>
@@ -1101,6 +1563,9 @@
       </c>
       <c r="G3" t="s">
         <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1140,13 +1605,13 @@
         <v>28</v>
       </c>
       <c r="D5" s="3">
-        <v>44032</v>
+        <v>44014</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1154,13 +1619,13 @@
         <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="3">
-        <v>44031</v>
+        <v>43960</v>
       </c>
       <c r="E6" t="s">
         <v>37</v>
@@ -1168,16 +1633,19 @@
       <c r="F6" t="s">
         <v>59</v>
       </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
         <v>70</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>71</v>
-      </c>
-      <c r="C7" t="s">
-        <v>72</v>
       </c>
       <c r="D7" s="3">
         <v>44030</v>
@@ -1188,22 +1656,28 @@
       <c r="F7" t="s">
         <v>3</v>
       </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
         <v>73</v>
-      </c>
-      <c r="C8" t="s">
-        <v>74</v>
       </c>
       <c r="D8" s="3">
         <v>44031</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
@@ -1214,10 +1688,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
         <v>28</v>
@@ -1240,16 +1714,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="3">
-        <v>44031</v>
+        <v>44001</v>
       </c>
       <c r="E10" t="s">
         <v>36</v>
@@ -1263,10 +1737,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
         <v>77</v>
-      </c>
-      <c r="B11" t="s">
-        <v>78</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
@@ -1286,10 +1760,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
         <v>28</v>
@@ -1309,33 +1783,33 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="3">
-        <v>44027</v>
+        <v>44017</v>
       </c>
       <c r="E13" t="s">
         <v>37</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="3">
         <v>44032</v>
@@ -1351,6 +1825,84 @@
       </c>
       <c r="H14" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="3">
+        <v>44033</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="3">
+        <v>44044</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="3">
+        <v>44041</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1362,8 +1914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>